<commit_message>
added page holders to reduce errors -SW
</commit_message>
<xml_diff>
--- a/BeerMeDB.xlsx
+++ b/BeerMeDB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-80" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Beer Category" sheetId="1" r:id="rId1"/>
@@ -1849,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1927,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>

</xml_diff>